<commit_message>
features analysed for 4 methods
</commit_message>
<xml_diff>
--- a/Dataset/feature_selection.xlsx
+++ b/Dataset/feature_selection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\CSE419\CSE419-Sensor-Data-based-Activity-Classification\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\NSU\CSE419\repository\CSE419-Sensor-Data-based-Activity-Classification\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DC7D09-47BB-4C93-97AC-27D44C4BA9F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE91DEF-0807-4515-B872-6EEE18716F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="77">
   <si>
     <t>lastSensorEventHours</t>
   </si>
@@ -228,9 +228,6 @@
     <t>with full dataset</t>
   </si>
   <si>
-    <t xml:space="preserve"> ar3ransitions</t>
-  </si>
-  <si>
     <t xml:space="preserve"> sensorCount-Chair</t>
   </si>
   <si>
@@ -255,14 +252,17 @@
     <t xml:space="preserve"> windowDuration</t>
   </si>
   <si>
-    <t>ar3ransitions</t>
+    <t>area transitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> area transitions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,13 +324,32 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -345,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -363,12 +382,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +677,7 @@
   <dimension ref="A1:AL29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,6 +686,7 @@
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="28" max="28" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -1122,233 +1148,232 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:38" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="N9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="R9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="S9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="U9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="V9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="W9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="X9" s="2" t="s">
+      <c r="X9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="Y9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="Z9" s="2" t="s">
+      <c r="Z9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AA9" s="2" t="s">
+      <c r="AA9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AB9" s="2" t="s">
+      <c r="AB9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AC9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AD9" s="2" t="s">
+      <c r="AD9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AE9" s="2" t="s">
+      <c r="AE9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AF9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AG9" s="2" t="s">
+      <c r="AG9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AH9" s="2" t="s">
+      <c r="AH9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AI9" s="2" t="s">
+      <c r="AI9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AJ9" s="2" t="s">
+      <c r="AJ9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AK9" s="2" t="s">
+      <c r="AK9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AL9" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="AL9" s="11"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N10" t="s">
-        <v>76</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="N10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="17"/>
+      <c r="P10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AG10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AH10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AI10" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AJ10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AJ10" t="s">
+      <c r="AK10" s="10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1356,106 +1381,108 @@
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="17"/>
+      <c r="P11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="R11" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="O11" t="s">
-        <v>23</v>
-      </c>
-      <c r="P11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="S11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="T11" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="R11" t="s">
-        <v>25</v>
-      </c>
-      <c r="S11" t="s">
+      <c r="U11" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="T11" t="s">
+      <c r="V11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="X11" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="U11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V11" t="s">
-        <v>49</v>
-      </c>
-      <c r="W11" t="s">
+      <c r="Y11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z11" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="X11" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y11" t="s">
+      <c r="AA11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE11" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="Z11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC11" t="s">
+      <c r="AF11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH11" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="AD11" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG11" t="s">
+      <c r="AI11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AJ11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AK11" s="10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1463,46 +1490,68 @@
       <c r="A12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G12" t="s">
+      <c r="E12" s="18"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J12" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M12" t="s">
+      <c r="W12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="N12" t="s">
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O12" t="s">
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="P12" t="s">
+      <c r="AD12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="AE12" s="18"/>
+      <c r="AF12" s="18"/>
+      <c r="AG12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="R12" t="s">
+      <c r="AH12" s="17"/>
+      <c r="AI12" s="18"/>
+      <c r="AJ12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="S12" t="s">
+      <c r="AK12" s="10" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1510,36 +1559,60 @@
       <c r="A13" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s">
-        <v>75</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="D13" s="17"/>
+      <c r="E13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="M13" t="s">
+      <c r="X13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="N13" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="P13" t="s">
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="18"/>
+      <c r="AG13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="AH13" s="17"/>
+      <c r="AI13" s="18"/>
+      <c r="AJ13" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="AK13" s="18"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>

</xml_diff>

<commit_message>
report added on meature selection
</commit_message>
<xml_diff>
--- a/Dataset/feature_selection.xlsx
+++ b/Dataset/feature_selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\NSU\CSE419\repository\CSE419-Sensor-Data-based-Activity-Classification\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE91DEF-0807-4515-B872-6EEE18716F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B384D65D-013C-4234-BAFD-F87BEAFDE66F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="83">
   <si>
     <t>lastSensorEventHours</t>
   </si>
@@ -256,13 +256,31 @@
   </si>
   <si>
     <t xml:space="preserve"> area transitions</t>
+  </si>
+  <si>
+    <t>about the locations</t>
+  </si>
+  <si>
+    <t>Original Set of Features</t>
+  </si>
+  <si>
+    <t>Selected Features with Low Variance Feature Removal</t>
+  </si>
+  <si>
+    <t>Selected Featured with L1 Based Feature Selection</t>
+  </si>
+  <si>
+    <t>Selected Features with Tree-based Feature Selection</t>
+  </si>
+  <si>
+    <t>Feature Selection with Random Forest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +349,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -364,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -394,6 +446,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,18 +740,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL29"/>
+  <dimension ref="A1:AL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
     <col min="28" max="28" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -693,6 +760,7 @@
       <c r="A1" t="s">
         <v>65</v>
       </c>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1583,7 +1651,6 @@
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
       <c r="U13" s="17"/>
@@ -1617,51 +1684,535 @@
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
+      <c r="K14" s="19" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="22"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="22"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="22"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="21"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="21"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="22"/>
+      <c r="E38" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="21"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>